<commit_message>
Conclusion from research about selected model
</commit_message>
<xml_diff>
--- a/documentation/models_to_evaluate.xlsx
+++ b/documentation/models_to_evaluate.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\RESEARCH\Hackaton_NLP_2024\SOURCE\SpanishMedicaLLM\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A4B9D2-C6DC-4A46-9C73-6E022987B842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DEDAAAC-2EC9-4F20-8E20-EC7EC8EE61E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List_of_models" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
   <si>
     <t>Description</t>
   </si>
@@ -60,11 +60,6 @@
     <t>LINCE-ZERO (Llm for Instructions from Natural Corpus en Español) is a Spanish instruction-tuned LLM 🔥
 			Developed by Clibrain, it is a causal decoder-only model with 7B parameters. LINCE-ZERO is based on Falcon-7B 
 			and has been fine-tuned using an 80k examples proprietary dataset inspired in famous instruction datasets such as Alpaca and Dolly.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	Versions:
-     Check the version quantized to 4 bits!
-       If you want to test the robust 40B parameters version called LINCE, you can request access at lince@clibrain.com.</t>
   </si>
   <si>
     <t>clibrain/Llama-2-7b-ft-instruct-es</t>
@@ -220,12 +215,84 @@
   <si>
     <t>Research Objetive:</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">	 Lo que significa que el pre-entrenamiento o entrenamiento base no es
+ completamente en espanol y si usa como base a Falcon-7B entonces es muy 
+ probable que el mayor conjunto de ejemplos que ha visto es en ingles</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.     </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Versions:
+     Check the version quantized to 4 bits!
+       If you want to test the robust 40B parameters version called LINCE, you can request access at lince@clibrain.com. </t>
+    </r>
+  </si>
+  <si>
+    <t>Pretrainin in Spanish</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/projecte-aina/aguila-7b</t>
+  </si>
+  <si>
+    <t>projecte-aina/aguila-7b</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Falcon-7B</t>
+  </si>
+  <si>
+    <t>Model description
+Ǎguila-7B is a transformer-based causal language model for Catalan, Spanish, and English. It is based on the Falcon-7B model and has been trained on a 26B token trilingual corpus collected from publicly available corpora and crawlers.
+More information available in the following post from Medium.com: Introducing Ǎguila, a new open-source LLM for Spanish and Catalan (https://medium.com/@mpamies247/introducing-a%CC%8Cguila-a-new-open-source-llm-for-spanish-and-catalan-ee1ebc70bc79)
+Intended uses and limitations
+The Ǎguila-7B model is ready-to-use only for causal language modeling to perform text-generation tasks. However, it is intended to be fine-tuned for downstream tasks.</t>
+  </si>
+  <si>
+    <t>Apache License, Version 2.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Language 	Percentage
+En 	16.84%
+Es 	41.38%
+Ca 	41.79%      https://medium.com/@mpamies247/introducing-a%CC%8Cguila-a-new-open-source-llm-for-spanish-and-catalan-ee1ebc70bc79</t>
+  </si>
+  <si>
+    <t>Este modelo se puede mezclar con BioMestral porque BioMistral fue entrenado tambien con español y tambien se puede usar la estrategia de Replay que propone Meditron</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -271,6 +338,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -293,7 +376,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -313,6 +396,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -594,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A5:G32"/>
+  <dimension ref="A5:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -605,13 +697,14 @@
     <col min="2" max="2" width="38.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.21875" customWidth="1"/>
-    <col min="6" max="6" width="28.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" customWidth="1"/>
+    <col min="6" max="6" width="46.21875" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>1</v>
@@ -623,78 +716,90 @@
         <v>6</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+    <row r="6" spans="1:8" s="2" customFormat="1" ht="288" x14ac:dyDescent="0.3">
+      <c r="A6" s="9">
+        <v>0</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="2" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
         <v>1</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" ht="171" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>2</v>
-      </c>
       <c r="B7" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>17</v>
+      <c r="F7" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="2" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="2" customFormat="1" ht="171" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="2" customFormat="1" ht="154.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:8" s="2" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
-        <v>4</v>
+        <v>1.5</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>4</v>
@@ -705,202 +810,224 @@
       <c r="D9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" s="2" customFormat="1" ht="178.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
+        <v>2</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
         <v>5</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="2" t="s">
+    </row>
+    <row r="12" spans="1:8" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
-        <v>6</v>
-      </c>
-      <c r="B11" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="2" customFormat="1" ht="172.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" s="2" customFormat="1" ht="114" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:8" s="2" customFormat="1" ht="172.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="F13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="2" customFormat="1" ht="114" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="2" customFormat="1" ht="233.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="2" t="s">
+    </row>
+    <row r="15" spans="1:8" s="2" customFormat="1" ht="233.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" s="3" t="s">
+    </row>
+    <row r="16" spans="1:8" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="C16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B15" s="2" t="s">
+      <c r="G16" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H16" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="2" t="s">
+    </row>
+    <row r="17" spans="2:8" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="H17" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="F21" s="6"/>
+    </row>
+    <row r="23" spans="2:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B23" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="8"/>
+    </row>
+    <row r="24" spans="2:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B24" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B16" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="E20" s="6"/>
-    </row>
-    <row r="22" spans="2:5" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B22" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="8"/>
-    </row>
-    <row r="23" spans="2:5" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B23" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="8"/>
-    </row>
-    <row r="24" spans="2:5" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B24" s="8"/>
       <c r="C24" s="8"/>
     </row>
-    <row r="25" spans="2:5" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
     </row>
-    <row r="26" spans="2:5" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
     </row>
-    <row r="27" spans="2:5" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B27" s="7" t="s">
+    <row r="27" spans="2:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+    </row>
+    <row r="28" spans="2:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B28" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="8"/>
+    </row>
+    <row r="29" spans="2:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B29" s="7"/>
+      <c r="C29" s="8"/>
+    </row>
+    <row r="30" spans="2:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B30" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="8"/>
+    </row>
+    <row r="31" spans="2:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B31" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" s="8"/>
+    </row>
+    <row r="32" spans="2:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B32" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="8"/>
+    </row>
+    <row r="33" spans="2:2" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B33" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="8"/>
-    </row>
-    <row r="28" spans="2:5" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B28" s="7"/>
-      <c r="C28" s="8"/>
-    </row>
-    <row r="29" spans="2:5" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B29" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29" s="8"/>
-    </row>
-    <row r="30" spans="2:5" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B30" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C30" s="8"/>
-    </row>
-    <row r="31" spans="2:5" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B31" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C31" s="8"/>
-    </row>
-    <row r="32" spans="2:5" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B32" s="8" t="s">
-        <v>53</v>
-      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:G16">
-    <sortCondition ref="A5:A16"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:H17">
+    <sortCondition ref="A5:A17"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="G6" r:id="rId1" xr:uid="{D91578FB-1D0C-43BE-BB95-1B7F0DE1452D}"/>
-    <hyperlink ref="G15" r:id="rId2" xr:uid="{7E930AF6-E7B2-4FF2-B119-5E999009953E}"/>
-    <hyperlink ref="G16" r:id="rId3" xr:uid="{BD8CD3A1-2D1F-4F0E-B5C8-5E65EA2485CC}"/>
+    <hyperlink ref="H7" r:id="rId1" xr:uid="{D91578FB-1D0C-43BE-BB95-1B7F0DE1452D}"/>
+    <hyperlink ref="H16" r:id="rId2" xr:uid="{7E930AF6-E7B2-4FF2-B119-5E999009953E}"/>
+    <hyperlink ref="H17" r:id="rId3" xr:uid="{BD8CD3A1-2D1F-4F0E-B5C8-5E65EA2485CC}"/>
+    <hyperlink ref="D6" r:id="rId4" display="https://www.apache.org/licenses/LICENSE-2.0" xr:uid="{07622A76-222C-4423-B7D1-4A2151006101}"/>
+    <hyperlink ref="G6" r:id="rId5" display="https://medium.com/@mpamies247/introducing-a%CC%8Cguila-a-new-open-source-llm-for-spanish-and-catalan-ee1ebc70bc79 Language _x0009_Percentage_x000a_En _x0009_16.84%_x000a_Es _x0009_41.38%_x000a_Ca _x0009_41.79%" xr:uid="{C8C4E330-FF0E-4544-ABC9-750996F4940C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Create information about finetuning approach for Model
</commit_message>
<xml_diff>
--- a/documentation/models_to_evaluate.xlsx
+++ b/documentation/models_to_evaluate.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\RESEARCH\Hackaton_NLP_2024\SOURCE\SpanishMedicaLLM\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F95AE60-95A0-4EF7-904C-C6F4006F68A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F28891-CC96-4B64-8488-BF4078A43FAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1236" yWindow="948" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List_of_models" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="64">
   <si>
     <t>Description</t>
   </si>
@@ -688,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A5:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1030,4 +1031,287 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CF62FF2-4D22-4424-93CA-8E10A1EAB95D}">
+  <dimension ref="B5:K17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:J17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="37.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B6" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="5"/>
+      <c r="H16" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H7" r:id="rId1" xr:uid="{1A63C700-EF17-4B2A-876C-BA9060A9FE07}"/>
+    <hyperlink ref="H16" r:id="rId2" xr:uid="{073FDBA5-2249-4775-9952-C7A53D516DD4}"/>
+    <hyperlink ref="H17" r:id="rId3" xr:uid="{EB1863B9-64A1-4B35-BBE4-D131E595C59A}"/>
+    <hyperlink ref="D6" r:id="rId4" display="https://www.apache.org/licenses/LICENSE-2.0" xr:uid="{1F37B5E9-2473-4C9E-9622-8F227C6B3F7F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>